<commit_message>
🐛 fix(docs): Modified files updated
Changes included (as of 2025-07-05 13:36:45):
- docs/project_management/comprehensive_report.xlsx: This file was modified with updates or fixes.
  Summary:
    diff --git a/docs/project_management/comprehensive_report.xlsx b/docs/project_management/comprehensive_report.xlsx
    index a3b0404..2af542a 100644
    Binary files a/docs/project_management/comprehensive_report.xlsx and b/docs/project_management/comprehensive_report.xlsx differ

Please describe the reason or issue addressed by these changes.
</commit_message>
<xml_diff>
--- a/docs/project_management/comprehensive_report.xlsx
+++ b/docs/project_management/comprehensive_report.xlsx
@@ -475,10 +475,10 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>383.66</v>
+        <v>365.38</v>
       </c>
       <c r="D2" t="n">
-        <v>348.03</v>
+        <v>335.55</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -497,10 +497,10 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>141.45</v>
+        <v>123.15</v>
       </c>
       <c r="D3" t="n">
-        <v>130.45</v>
+        <v>141.41</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -519,10 +519,10 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>117.25</v>
+        <v>128.3</v>
       </c>
       <c r="D4" t="n">
-        <v>123.58</v>
+        <v>89.16</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -541,10 +541,10 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>124.95</v>
+        <v>113.93</v>
       </c>
       <c r="D5" t="n">
-        <v>94</v>
+        <v>104.98</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -563,10 +563,10 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>69.44</v>
+        <v>67.31</v>
       </c>
       <c r="D6" t="n">
-        <v>68.91</v>
+        <v>64</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>72.01000000000001</v>
+        <v>73.20999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>61.54</v>
+        <v>45.25</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -607,10 +607,10 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>64.98999999999999</v>
+        <v>55.84</v>
       </c>
       <c r="D8" t="n">
-        <v>58.45</v>
+        <v>77.41</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -629,10 +629,10 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>61.83</v>
+        <v>66.41</v>
       </c>
       <c r="D9" t="n">
-        <v>52.76</v>
+        <v>52.57</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -651,10 +651,10 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
-        <v>63.12</v>
+        <v>61.9</v>
       </c>
       <c r="D10" t="n">
-        <v>41.24</v>
+        <v>36.58</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -673,10 +673,10 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>52.26</v>
+        <v>40.72</v>
       </c>
       <c r="D11" t="n">
-        <v>65.13</v>
+        <v>59.73</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🐛 fix(docs): Modified files updated\n\nChanges included (as of 2025-07-05 16:44:56):\n- docs/project_management/comprehensive_report.xlsx: This file was modified with updates or fixes.\n  Summary:\n    diff --git a/docs/project_management/comprehensive_report.xlsx b/docs/project_management/comprehensive_report.xlsx\n    index a3b0404..f9a964c 100644\n    Binary files a/docs/project_management/comprehensive_report.xlsx and b/docs/project_management/comprehensive_report.xlsx differ\n\n\nPlease describe the reason or issue addressed by these changes.
</commit_message>
<xml_diff>
--- a/docs/project_management/comprehensive_report.xlsx
+++ b/docs/project_management/comprehensive_report.xlsx
@@ -427,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
@@ -475,10 +475,10 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>383.66</v>
+        <v>402.04</v>
       </c>
       <c r="D2" t="n">
-        <v>348.03</v>
+        <v>350.3</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -497,10 +497,10 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>141.45</v>
+        <v>128.15</v>
       </c>
       <c r="D3" t="n">
-        <v>130.45</v>
+        <v>114.1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -519,10 +519,10 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>117.25</v>
+        <v>53.04</v>
       </c>
       <c r="D4" t="n">
-        <v>123.58</v>
+        <v>55.28</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -541,10 +541,10 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>124.95</v>
+        <v>75.11</v>
       </c>
       <c r="D5" t="n">
-        <v>94</v>
+        <v>58.82</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -563,10 +563,10 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>69.44</v>
+        <v>114.85</v>
       </c>
       <c r="D6" t="n">
-        <v>68.91</v>
+        <v>113.28</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -585,10 +585,10 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>72.01000000000001</v>
+        <v>57.11</v>
       </c>
       <c r="D7" t="n">
-        <v>61.54</v>
+        <v>56.05</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -607,10 +607,10 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>64.98999999999999</v>
+        <v>57.75</v>
       </c>
       <c r="D8" t="n">
-        <v>58.45</v>
+        <v>57.22</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -629,10 +629,10 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>61.83</v>
+        <v>159.04</v>
       </c>
       <c r="D9" t="n">
-        <v>52.76</v>
+        <v>122.93</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -651,10 +651,10 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
-        <v>63.12</v>
+        <v>82.59999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>41.24</v>
+        <v>65.98</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -673,10 +673,10 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>52.26</v>
+        <v>76.44</v>
       </c>
       <c r="D11" t="n">
-        <v>65.13</v>
+        <v>56.95</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>

</xml_diff>